<commit_message>
Init seasonality study and AWS s3 pulls
</commit_message>
<xml_diff>
--- a/DataFeeds/Ben_Predictions.xlsx
+++ b/DataFeeds/Ben_Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpMeesam\Dev\Canpotex\DataFeeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89B800A-8819-46EA-A531-9CACC566A05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA046A8-644A-4D3B-B59C-A473EF63049C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AC99038-628D-430C-B1D7-95B3A94606CB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6AC99038-628D-430C-B1D7-95B3A94606CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -115,6 +121,8 @@
     <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="6" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,12 +440,12 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44440</v>
       </c>
@@ -466,7 +474,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44470</v>
       </c>
@@ -487,7 +495,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44501</v>
       </c>
@@ -508,7 +516,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44531</v>
       </c>
@@ -529,7 +537,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44562</v>
       </c>
@@ -550,7 +558,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44593</v>
       </c>
@@ -571,7 +579,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44621</v>
       </c>
@@ -592,7 +600,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44652</v>
       </c>
@@ -613,7 +621,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44682</v>
       </c>
@@ -634,7 +642,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44713</v>
       </c>
@@ -655,7 +663,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44743</v>
       </c>
@@ -676,7 +684,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44774</v>
       </c>
@@ -697,8 +705,13 @@
       <c r="N13" s="2"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
+        <v>44805</v>
+      </c>
+      <c r="B14" s="9">
+        <v>742.53</v>
+      </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -713,10 +726,32 @@
       <c r="N14" s="2"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
+        <v>44835</v>
+      </c>
+      <c r="B15" s="9">
+        <v>793.14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
+        <v>44866</v>
+      </c>
+      <c r="B16" s="9">
+        <v>795.77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>44896</v>
+      </c>
+      <c r="B17" s="9">
+        <v>798.62</v>
+      </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C18" s="7"/>
     </row>
   </sheetData>

</xml_diff>